<commit_message>
Updated list of top 20 DEG for all programs
</commit_message>
<xml_diff>
--- a/Top20DEG_allPrograms.xlsx
+++ b/Top20DEG_allPrograms.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="15000" yWindow="540" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="75">
   <si>
     <t>logFC</t>
   </si>
@@ -32,66 +33,6 @@
     <t>PValue</t>
   </si>
   <si>
-    <t>MSTRG.12806.3</t>
-  </si>
-  <si>
-    <t>MSTRG.3861.2</t>
-  </si>
-  <si>
-    <t>MSTRG.11443.10</t>
-  </si>
-  <si>
-    <t>MSTRG.5023.2</t>
-  </si>
-  <si>
-    <t>hxAUG25s14g268t1</t>
-  </si>
-  <si>
-    <t>MSTRG.1892.1</t>
-  </si>
-  <si>
-    <t>MSTRG.15387.3</t>
-  </si>
-  <si>
-    <t>hxAUG26up1s9g220t1</t>
-  </si>
-  <si>
-    <t>MSTRG.14970.2</t>
-  </si>
-  <si>
-    <t>hxAUG25s18g143t1</t>
-  </si>
-  <si>
-    <t>MSTRG.3568.4</t>
-  </si>
-  <si>
-    <t>MSTRG.17777.1</t>
-  </si>
-  <si>
-    <t>hxAUG26res20g117t1</t>
-  </si>
-  <si>
-    <t>hxAUG25s18g144t1</t>
-  </si>
-  <si>
-    <t>hxAUG26us18g89t1</t>
-  </si>
-  <si>
-    <t>hxNCBI_GNO_104203</t>
-  </si>
-  <si>
-    <t>MSTRG.14309.8</t>
-  </si>
-  <si>
-    <t>hxAUG25s13g409t1</t>
-  </si>
-  <si>
-    <t>hxAUG26res724g88t1</t>
-  </si>
-  <si>
-    <t>MSTRG.17787.2</t>
-  </si>
-  <si>
     <t>Program</t>
   </si>
   <si>
@@ -282,13 +223,40 @@
   </si>
   <si>
     <t>DESeq</t>
+  </si>
+  <si>
+    <t>MSTRG.6850</t>
+  </si>
+  <si>
+    <t>MSTRG.5768</t>
+  </si>
+  <si>
+    <t>hxAUG26res20g199t1</t>
+  </si>
+  <si>
+    <t>MSTRG.6670</t>
+  </si>
+  <si>
+    <t>MSTRG.13640</t>
+  </si>
+  <si>
+    <t>MSTRG.6204</t>
+  </si>
+  <si>
+    <t>MSTRG.3797</t>
+  </si>
+  <si>
+    <t>MSTRG.6233</t>
+  </si>
+  <si>
+    <t>MSTRG.5769</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -296,8 +264,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +300,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -326,21 +316,85 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="5">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -613,7 +667,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D81"/>
+  <dimension ref="A1:D80"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -623,15 +677,18 @@
     <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" customWidth="1"/>
     <col min="16" max="16" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -641,1126 +698,1488 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
+      <c r="A2" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C2">
-        <v>14.3055848089704</v>
+        <v>8.4418560428744893</v>
       </c>
       <c r="D2" s="1">
-        <v>1.10170600175108E-24</v>
+        <v>5.4291040863456105E-57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>3</v>
+      <c r="A3" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C3">
-        <v>-13.814879656238899</v>
+        <v>-7.5703070369659002</v>
       </c>
       <c r="D3" s="1">
-        <v>2.0864467262009E-24</v>
+        <v>1.18059385650559E-56</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
       <c r="C4">
-        <v>-13.3485282386384</v>
+        <v>-11.000510966984301</v>
       </c>
       <c r="D4" s="1">
-        <v>2.8876916561865399E-22</v>
+        <v>4.81991508772126E-48</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>5</v>
+      <c r="A5" t="s">
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>-13.1859054222406</v>
+        <v>-11.6257307664024</v>
       </c>
       <c r="D5" s="1">
-        <v>9.6673463868354607E-22</v>
+        <v>1.40024192369858E-46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
+      <c r="A6" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>-11.534091944174801</v>
+        <v>-5.8220035488317103</v>
       </c>
       <c r="D6" s="1">
-        <v>7.5173786313706703E-21</v>
+        <v>2.2077852898605401E-41</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>29</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C7">
-        <v>12.035745428189699</v>
+        <v>-5.9810032101124602</v>
       </c>
       <c r="D7" s="1">
-        <v>9.12799672849251E-21</v>
+        <v>2.98813036809709E-35</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>8</v>
+      <c r="A8" t="s">
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>12.4410017115739</v>
+        <v>-7.9528379251875601</v>
       </c>
       <c r="D8" s="1">
-        <v>2.0775863128262899E-17</v>
+        <v>7.9590352154443305E-35</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>9</v>
+      <c r="A9" t="s">
+        <v>68</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>-7.4167327767950404</v>
+        <v>-9.4359931994218496</v>
       </c>
       <c r="D9" s="1">
-        <v>2.23529112181435E-17</v>
+        <v>1.32790088868757E-29</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>10</v>
+      <c r="A10" t="s">
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C10">
-        <v>-12.1809459252453</v>
+        <v>-5.8673632107211597</v>
       </c>
       <c r="D10" s="1">
-        <v>7.1408766679629905E-17</v>
+        <v>1.38594266667185E-29</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>11</v>
+      <c r="A11" t="s">
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C11">
-        <v>-8.0023526235294309</v>
+        <v>-6.9342903118787103</v>
       </c>
       <c r="D11" s="1">
-        <v>1.2441144287047001E-15</v>
+        <v>1.8068342011271599E-29</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C12">
-        <v>-9.51386935901232</v>
+        <v>-7.7934939957018097</v>
       </c>
       <c r="D12" s="1">
-        <v>3.9838983515543899E-14</v>
+        <v>2.5566908447376202E-29</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>13</v>
+      <c r="A13" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>-11.6518179008257</v>
+        <v>-6.5350216470264897</v>
       </c>
       <c r="D13" s="1">
-        <v>7.8452526928030896E-14</v>
+        <v>6.85337546953189E-29</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>14</v>
+      <c r="A14" s="6" t="s">
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>-11.457444706877901</v>
+        <v>-3.9058466576758302</v>
       </c>
       <c r="D14" s="1">
-        <v>7.7835226286561202E-13</v>
+        <v>1.4858073364523199E-27</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="3" t="s">
-        <v>15</v>
+      <c r="A15" t="s">
+        <v>70</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>-7.4866770290870397</v>
+        <v>-7.0349030532399297</v>
       </c>
       <c r="D15" s="1">
-        <v>1.7227338445755001E-12</v>
+        <v>4.1152365316797102E-27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
-        <v>16</v>
+      <c r="A16" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>-5.9088003324124596</v>
+        <v>-4.0801389370021601</v>
       </c>
       <c r="D16" s="1">
-        <v>1.8595548031660399E-12</v>
+        <v>6.3175775696232202E-27</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="3" t="s">
-        <v>17</v>
+      <c r="A17" t="s">
+        <v>71</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>-7.9117865842157702</v>
+        <v>11.4831477558362</v>
       </c>
       <c r="D17" s="1">
-        <v>4.54623274117219E-12</v>
+        <v>1.7319979610570201E-25</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="3" t="s">
-        <v>18</v>
+      <c r="A18" t="s">
+        <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C18">
-        <v>-12.263223606206999</v>
+        <v>-8.4629662574573707</v>
       </c>
       <c r="D18" s="1">
-        <v>8.0705692751307794E-12</v>
+        <v>3.8286830134687099E-25</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="3" t="s">
-        <v>19</v>
+      <c r="A19" t="s">
+        <v>72</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C19">
-        <v>-6.85283544957373</v>
+        <v>-9.5957025564495897</v>
       </c>
       <c r="D19" s="1">
-        <v>1.31464185631577E-11</v>
+        <v>2.5277848620480699E-24</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
-        <v>20</v>
+      <c r="A20" t="s">
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C20">
-        <v>-11.017912202871701</v>
+        <v>-3.40670653202762</v>
       </c>
       <c r="D20" s="1">
-        <v>1.6306752227818199E-11</v>
+        <v>4.4924243854408498E-24</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>21</v>
+      <c r="A21" t="s">
+        <v>74</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C21">
-        <v>9.0651841418729298</v>
+        <v>-7.4458382054845602</v>
       </c>
       <c r="D21" s="1">
-        <v>2.7092782815719202E-11</v>
+        <v>1.55942287432941E-23</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C22">
-        <v>-6.0779706037275503</v>
-      </c>
-      <c r="D22" s="1">
-        <v>3.0600000000000003E-8</v>
+        <v>-7.3826740506989497</v>
+      </c>
+      <c r="D22">
+        <v>1.9984362903192001E-157</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C23">
-        <v>-6.8600375217428002</v>
-      </c>
-      <c r="D23" s="1">
-        <v>1.15E-7</v>
+        <v>-5.7770188095579904</v>
+      </c>
+      <c r="D23">
+        <v>7.3027739575009004E-72</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5" t="s">
-        <v>27</v>
+      <c r="A24" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C24">
-        <v>-5.7723374319816401</v>
-      </c>
-      <c r="D24" s="1">
-        <v>2.0100000000000001E-7</v>
+        <v>7.8669918307913598</v>
+      </c>
+      <c r="D24">
+        <v>4.6450935929637099E-58</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="3" t="s">
-        <v>28</v>
+      <c r="A25" s="6" t="s">
+        <v>51</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C25">
-        <v>-1.8022059976379901</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1.7599999999999999E-7</v>
+        <v>-5.5955106285160303</v>
+      </c>
+      <c r="D25">
+        <v>2.9241073118836802E-57</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
-        <v>29</v>
+      <c r="A26" t="s">
+        <v>52</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C26">
-        <v>0.56280048204135802</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1.6899999999999999E-7</v>
+        <v>-7.3924853082235797</v>
+      </c>
+      <c r="D26">
+        <v>1.06918344071471E-55</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C27">
-        <v>2.0448856894038299</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3.3500000000000002E-7</v>
+        <v>2.27778639634673</v>
+      </c>
+      <c r="D27">
+        <v>2.0010747813168301E-52</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C28">
-        <v>-4.2364600279932398</v>
-      </c>
-      <c r="D28" s="1">
-        <v>3.9400000000000001E-7</v>
+        <v>-5.6066679479869901</v>
+      </c>
+      <c r="D28">
+        <v>6.50131569415447E-51</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>32</v>
+      <c r="A29" t="s">
+        <v>54</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C29">
-        <v>-1.6895295499166101</v>
-      </c>
-      <c r="D29" s="1">
-        <v>6.0100000000000005E-7</v>
+        <v>1.75850465486232</v>
+      </c>
+      <c r="D29">
+        <v>4.8214941561114699E-49</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>45</v>
+        <v>65</v>
       </c>
       <c r="C30">
-        <v>-0.45704356364158</v>
-      </c>
-      <c r="D30" s="1">
-        <v>7.9400000000000004E-7</v>
+        <v>-7.16164596286806</v>
+      </c>
+      <c r="D30">
+        <v>5.4761464497761799E-46</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31">
+        <v>3.4059405320998599</v>
+      </c>
+      <c r="D31">
+        <v>1.74321305214096E-45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32">
+        <v>-1.9647866251424999</v>
+      </c>
+      <c r="D32">
+        <v>3.69471766573877E-41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33">
+        <v>-3.7943252882983902</v>
+      </c>
+      <c r="D33">
+        <v>4.2402497899471498E-41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34">
+        <v>-6.1035214678760896</v>
+      </c>
+      <c r="D34">
+        <v>1.10344370647554E-40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B35" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35">
+        <v>-3.9590710377740899</v>
+      </c>
+      <c r="D35">
+        <v>1.36911383206092E-40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36">
+        <v>3.8507889328171498</v>
+      </c>
+      <c r="D36">
+        <v>1.76377329679445E-40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>60</v>
+      </c>
+      <c r="B37" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37">
+        <v>-4.0893643449328296</v>
+      </c>
+      <c r="D37">
+        <v>1.3630101037103499E-38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>61</v>
+      </c>
+      <c r="B38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38">
+        <v>-3.3218271846985798</v>
+      </c>
+      <c r="D38">
+        <v>2.1606802169035801E-38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" t="s">
+        <v>65</v>
+      </c>
+      <c r="C39">
+        <v>1.10822887144077</v>
+      </c>
+      <c r="D39">
+        <v>2.0788486470316199E-38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B40" t="s">
+        <v>65</v>
+      </c>
+      <c r="C40">
+        <v>2.03759109871406</v>
+      </c>
+      <c r="D40">
+        <v>2.0501269541679699E-38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="1">
+        <v>3.0681913676389198E-8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
         <v>34</v>
       </c>
-      <c r="B31" t="s">
-        <v>45</v>
-      </c>
-      <c r="C31">
-        <v>-5.0924427832664296</v>
-      </c>
-      <c r="D31" s="1">
-        <v>9.5300000000000002E-7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
+      <c r="D42" s="1">
+        <v>1.15633969177686E-7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
         <v>35</v>
       </c>
-      <c r="B32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C32">
-        <v>0.85230430637445498</v>
-      </c>
-      <c r="D32" s="1">
-        <v>1.13E-6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
+      <c r="D43" s="1">
+        <v>2.0200686812188501E-7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
         <v>36</v>
       </c>
-      <c r="B33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33">
-        <v>0.36597867789564098</v>
-      </c>
-      <c r="D33" s="1">
-        <v>1.31E-6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A34" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34">
-        <v>-0.79873070327500395</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1.64E-6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35">
-        <v>3.96542431370621</v>
-      </c>
-      <c r="D35" s="1">
-        <v>2.0700000000000001E-6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36">
-        <v>-2.6112773267620599</v>
-      </c>
-      <c r="D36" s="1">
-        <v>2.7499999999999999E-6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37">
-        <v>-0.96946540601347797</v>
-      </c>
-      <c r="D37" s="1">
-        <v>3.32E-6</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A38" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B38" t="s">
-        <v>45</v>
-      </c>
-      <c r="C38">
-        <v>-5.2302729955824603</v>
-      </c>
-      <c r="D38" s="1">
-        <v>3.8199999999999998E-6</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39">
-        <v>1.7924352640502601</v>
-      </c>
-      <c r="D39" s="1">
-        <v>4.0099999999999997E-6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A40" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40" t="s">
-        <v>45</v>
-      </c>
-      <c r="C40">
-        <v>1.9319387019555201</v>
-      </c>
-      <c r="D40" s="1">
-        <v>3.6799999999999999E-6</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" t="s">
-        <v>45</v>
-      </c>
-      <c r="C41">
-        <v>-0.71386963624124899</v>
-      </c>
-      <c r="D41" s="1">
-        <v>4.2300000000000002E-6</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" t="s">
-        <v>53</v>
-      </c>
-      <c r="D42" s="1">
-        <v>3.0681913676389198E-8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B43" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D43" s="1">
-        <v>1.15633969177686E-7</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" t="s">
-        <v>55</v>
-      </c>
       <c r="D44" s="1">
-        <v>2.0200686812188501E-7</v>
+        <v>1.76006792695915E-7</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="B45" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C45" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="D45" s="1">
-        <v>1.76006792695915E-7</v>
+        <v>1.6844008277061599E-7</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D46" s="1">
-        <v>1.6844008277061599E-7</v>
+        <v>3.3515715158749499E-7</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B47" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D47" s="1">
-        <v>3.3515715158749499E-7</v>
+        <v>3.9503888960013001E-7</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="D48" s="1">
-        <v>3.9503888960013001E-7</v>
+        <v>6.0218617559115696E-7</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C49" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="D49" s="1">
-        <v>6.0218617559115696E-7</v>
+        <v>7.9692858157010004E-7</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
-        <v>48</v>
+        <v>29</v>
       </c>
       <c r="B50" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D50" s="1">
-        <v>7.9692858157010004E-7</v>
+        <v>9.5547884060298592E-7</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D51" s="1">
-        <v>9.5547884060298592E-7</v>
+        <v>1.1298171307405599E-6</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B52" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="D52" s="1">
-        <v>1.1298171307405599E-6</v>
+        <v>1.3169142403235399E-6</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="B53" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C53" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="D53" s="1">
-        <v>1.3169142403235399E-6</v>
+        <v>1.6496922894404501E-6</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
-        <v>51</v>
+        <v>18</v>
       </c>
       <c r="B54" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C54" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="D54" s="1">
-        <v>1.6496922894404501E-6</v>
+        <v>2.0667662009587998E-6</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B55" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="D55" s="1">
-        <v>2.0667662009587998E-6</v>
+        <v>2.75241734815079E-6</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B56" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D56" s="1">
-        <v>2.75241734815079E-6</v>
+        <v>3.31559538013781E-6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B57" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C57" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="D57" s="1">
-        <v>3.31559538013781E-6</v>
+        <v>3.8291136930101999E-6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="B58" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C58" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="D58" s="1">
-        <v>3.8291136930101999E-6</v>
+        <v>4.0137393353401103E-6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="B59" t="s">
-        <v>23</v>
-      </c>
-      <c r="C59" t="s">
-        <v>70</v>
+        <v>3</v>
+      </c>
+      <c r="C59" s="2">
+        <v>1.9320165364155499</v>
       </c>
       <c r="D59" s="1">
-        <v>4.0137393353401103E-6</v>
+        <v>3.6852798555031498E-6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B60" t="s">
-        <v>23</v>
+        <v>3</v>
       </c>
       <c r="C60" s="2">
-        <v>1.9320165364155499</v>
+        <v>-0.71381078844205303</v>
       </c>
       <c r="D60" s="1">
-        <v>3.6852798555031498E-6</v>
+        <v>4.2598650544789498E-6</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="3" t="s">
-        <v>44</v>
+      <c r="A61" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B61" t="s">
-        <v>23</v>
-      </c>
-      <c r="C61" s="2">
-        <v>-0.71381078844205303</v>
+        <v>25</v>
+      </c>
+      <c r="C61">
+        <v>-6.0779706037275503</v>
       </c>
       <c r="D61" s="1">
-        <v>4.2598650544789498E-6</v>
+        <v>3.0600000000000003E-8</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
         <v>25</v>
       </c>
-      <c r="B62" t="s">
-        <v>85</v>
-      </c>
       <c r="C62">
-        <v>-7.3826740506989497</v>
-      </c>
-      <c r="D62">
-        <v>1.9984362903192001E-157</v>
+        <v>-6.8600375217428002</v>
+      </c>
+      <c r="D62" s="1">
+        <v>1.15E-7</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
-        <v>34</v>
+      <c r="A63" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C63">
-        <v>-5.7770188095579904</v>
-      </c>
-      <c r="D63">
-        <v>7.3027739575009004E-72</v>
+        <v>-5.7723374319816401</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2.0100000000000001E-7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C64">
-        <v>7.8669918307913598</v>
-      </c>
-      <c r="D64">
-        <v>4.6450935929637099E-58</v>
+        <v>-1.8022059976379901</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1.7599999999999999E-7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>71</v>
+      <c r="A65" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C65">
-        <v>-5.5955106285160303</v>
-      </c>
-      <c r="D65">
-        <v>2.9241073118836802E-57</v>
+        <v>0.56280048204135802</v>
+      </c>
+      <c r="D65" s="1">
+        <v>1.6899999999999999E-7</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>72</v>
+      <c r="A66" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="B66" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C66">
-        <v>-7.3924853082235797</v>
-      </c>
-      <c r="D66">
-        <v>1.06918344071471E-55</v>
+        <v>2.0448856894038299</v>
+      </c>
+      <c r="D66" s="1">
+        <v>3.3500000000000002E-7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
-        <v>43</v>
+      <c r="A67" t="s">
+        <v>11</v>
       </c>
       <c r="B67" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C67">
-        <v>2.27778639634673</v>
-      </c>
-      <c r="D67">
-        <v>2.0010747813168301E-52</v>
+        <v>-4.2364600279932398</v>
+      </c>
+      <c r="D67" s="1">
+        <v>3.9400000000000001E-7</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
-        <v>73</v>
+      <c r="A68" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="B68" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C68">
-        <v>-5.6066679479869901</v>
-      </c>
-      <c r="D68">
-        <v>6.50131569415447E-51</v>
+        <v>-1.6895295499166101</v>
+      </c>
+      <c r="D68" s="1">
+        <v>6.0100000000000005E-7</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
-        <v>74</v>
+      <c r="A69" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="B69" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C69">
-        <v>1.75850465486232</v>
-      </c>
-      <c r="D69">
-        <v>4.8214941561114699E-49</v>
+        <v>-0.45704356364158</v>
+      </c>
+      <c r="D69" s="1">
+        <v>7.9400000000000004E-7</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="5" t="s">
-        <v>27</v>
+      <c r="A70" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="B70" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C70">
-        <v>-7.16164596286806</v>
-      </c>
-      <c r="D70">
-        <v>5.4761464497761799E-46</v>
+        <v>-5.0924427832664296</v>
+      </c>
+      <c r="D70" s="1">
+        <v>9.5300000000000002E-7</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C71">
-        <v>3.4059405320998599</v>
-      </c>
-      <c r="D71">
-        <v>1.74321305214096E-45</v>
+        <v>0.85230430637445498</v>
+      </c>
+      <c r="D71" s="1">
+        <v>1.13E-6</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>75</v>
+      <c r="A72" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C72">
-        <v>-1.9647866251424999</v>
-      </c>
-      <c r="D72">
-        <v>3.69471766573877E-41</v>
+        <v>0.36597867789564098</v>
+      </c>
+      <c r="D72" s="1">
+        <v>1.31E-6</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
-        <v>76</v>
+      <c r="A73" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C73">
-        <v>-3.7943252882983902</v>
-      </c>
-      <c r="D73">
-        <v>4.2402497899471498E-41</v>
+        <v>-0.79873070327500395</v>
+      </c>
+      <c r="D73" s="1">
+        <v>1.64E-6</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>77</v>
+      <c r="A74" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="B74" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C74">
-        <v>-6.1035214678760896</v>
-      </c>
-      <c r="D74">
-        <v>1.10344370647554E-40</v>
+        <v>3.96542431370621</v>
+      </c>
+      <c r="D74" s="1">
+        <v>2.0700000000000001E-6</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>78</v>
+      <c r="A75" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="B75" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C75">
-        <v>-3.9590710377740899</v>
-      </c>
-      <c r="D75">
-        <v>1.36911383206092E-40</v>
+        <v>-2.6112773267620599</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2.7499999999999999E-6</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>79</v>
+      <c r="A76" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C76">
-        <v>3.8507889328171498</v>
-      </c>
-      <c r="D76">
-        <v>1.76377329679445E-40</v>
+        <v>-0.96946540601347797</v>
+      </c>
+      <c r="D76" s="1">
+        <v>3.32E-6</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>80</v>
+      <c r="A77" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="B77" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C77">
-        <v>-4.0893643449328296</v>
-      </c>
-      <c r="D77">
-        <v>1.3630101037103499E-38</v>
+        <v>-5.2302729955824603</v>
+      </c>
+      <c r="D77" s="1">
+        <v>3.8199999999999998E-6</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>81</v>
+      <c r="A78" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C78">
-        <v>-3.3218271846985798</v>
-      </c>
-      <c r="D78">
-        <v>2.1606802169035801E-38</v>
+        <v>1.7924352640502601</v>
+      </c>
+      <c r="D78" s="1">
+        <v>4.0099999999999997E-6</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
-        <v>82</v>
+      <c r="A79" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="B79" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C79">
-        <v>1.10822887144077</v>
-      </c>
-      <c r="D79">
-        <v>2.0788486470316199E-38</v>
+        <v>1.9319387019555201</v>
+      </c>
+      <c r="D79" s="1">
+        <v>3.6799999999999999E-6</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" t="s">
-        <v>83</v>
+      <c r="A80" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B80" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="C80">
-        <v>2.03759109871406</v>
-      </c>
-      <c r="D80">
-        <v>2.0501269541679699E-38</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" t="s">
-        <v>84</v>
-      </c>
-      <c r="B81" t="s">
-        <v>85</v>
-      </c>
-      <c r="C81">
-        <v>1.6489933631826299</v>
-      </c>
-      <c r="D81">
-        <v>1.8128253668817299E-36</v>
+        <v>-0.71386963624124899</v>
+      </c>
+      <c r="D80" s="1">
+        <v>4.2300000000000002E-6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="A1:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" t="s">
+        <v>60</v>
+      </c>
+      <c r="E17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>62</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" t="s">
+        <v>64</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>